<commit_message>
Avances desafrio n3 pre entrega
</commit_message>
<xml_diff>
--- a/Desafio2_Casos de prueba/CasosDePrueba_SantiagoAguirre.xlsx
+++ b/Desafio2_Casos de prueba/CasosDePrueba_SantiagoAguirre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santi\Desktop\CODERHOUSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAGUIRRE\Documents\GitHub\CODERHOUSE\Desafio2_Casos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{508E9CEB-A24A-4FD9-BFB0-EA03BAE7FA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48119F0B-FD0B-453C-A11E-E38B47813C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-60" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos y ejecuciones" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="133">
   <si>
     <t xml:space="preserve">Id </t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Estar logueado</t>
-  </si>
-  <si>
-    <t>PS_002</t>
   </si>
   <si>
     <t>Negativo</t>
@@ -302,21 +299,12 @@
     <t>La pagina hotels no funciona</t>
   </si>
   <si>
-    <t>Imposibilidad de ingresar NUMEROS como Nombre al registrarse</t>
-  </si>
-  <si>
-    <t>Verificar que no sea posible ingresar numeros en el campo First Name, al registrarse</t>
-  </si>
-  <si>
     <t>1- 12345</t>
   </si>
   <si>
     <t>2- Last name: Gimenez</t>
   </si>
   <si>
-    <t>3- 1145879587</t>
-  </si>
-  <si>
     <t>4- gimenes@gmail.com</t>
   </si>
   <si>
@@ -344,12 +332,6 @@
     <t>11 - Confirm password: santiago123</t>
   </si>
   <si>
-    <t>Ingresar los datos de entrada indicados, ingresando 12345 en First Name</t>
-  </si>
-  <si>
-    <t>Obtengo un popup, que me indica la necesidad de ingresar un nombre valido.</t>
-  </si>
-  <si>
     <t>La pagina acepta los numeros como nombre y registra al cliente</t>
   </si>
   <si>
@@ -395,18 +377,9 @@
     <t>La pagina rechaza el inicio de sesión correctamente</t>
   </si>
   <si>
-    <t>Funcionamiento de area de Ayuda</t>
-  </si>
-  <si>
-    <t>Verificar el correcto funcionamiento del enlace SUPPORT</t>
-  </si>
-  <si>
     <t>Hacer click en support, ubicado en el margen superior de la página</t>
   </si>
   <si>
-    <t>Debería poderse ingresar al area de soporte, y visualizar los links y telefonos de contacto de la empresa.</t>
-  </si>
-  <si>
     <t>La pagina no funciona.</t>
   </si>
   <si>
@@ -438,6 +411,27 @@
   </si>
   <si>
     <t xml:space="preserve">No se puede ingresar al enlace, debido a que la pagina está caída o en construcción. </t>
+  </si>
+  <si>
+    <t>PS-002</t>
+  </si>
+  <si>
+    <t>Debería poderse ingresar al area de CONTACTO, y visualizar los links y telefonos de contacto de la empresa.</t>
+  </si>
+  <si>
+    <t>Imposibilidad de ingresar LETRAS como numero de telefono al registrarse</t>
+  </si>
+  <si>
+    <t>Verificar que no sea posible ingresar letras en el campo telefono al registrarse.</t>
+  </si>
+  <si>
+    <t>Ingresar los datos de entrada indicados, ingresando AAA en Telefono</t>
+  </si>
+  <si>
+    <t>3-Telefono: AAA</t>
+  </si>
+  <si>
+    <t>Obtengo un popup, que me indica la necesidad de ingresar un numero de telefono valido.</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1404,53 +1398,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1508,255 +1455,386 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1975,9 +2053,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:L990"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2032,1486 +2110,1486 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="102" t="s">
+      <c r="C4" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="56"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="58">
+        <v>1</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="138" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="139" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="32.25" customHeight="1">
+      <c r="A5" s="60"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="64">
+        <v>2</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="60"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+    </row>
+    <row r="7" spans="1:12" ht="35.25" customHeight="1">
+      <c r="A7" s="60"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="68"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="60"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+    </row>
+    <row r="9" spans="1:12" ht="38.25" customHeight="1" thickBot="1">
+      <c r="A9" s="49"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="76"/>
+      <c r="C10" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="63"/>
+      <c r="G10" s="79">
+        <v>1</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="103" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10">
+      <c r="K10" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="140" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45">
+      <c r="A11" s="60"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="82">
+        <v>2</v>
+      </c>
+      <c r="H11" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="101"/>
+      <c r="L11" s="36"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="60"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="101"/>
+      <c r="L12" s="36"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="60"/>
+      <c r="B13" s="86" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="101"/>
+      <c r="L13" s="36"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="60"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="36"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="60"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="36"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="60"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="36"/>
+    </row>
+    <row r="17" spans="1:12" ht="7.5" customHeight="1" thickBot="1">
+      <c r="A17" s="60"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="101"/>
+      <c r="L17" s="36"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A18" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="92" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="58">
         <v>1</v>
       </c>
-      <c r="H4" s="80" t="s">
+      <c r="H18" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="141" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="142" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A19" s="60"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="64">
+        <v>2</v>
+      </c>
+      <c r="H19" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="84" t="s">
+      <c r="I19" s="39"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="143"/>
+      <c r="L19" s="61"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A20" s="60"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="65">
+        <v>3</v>
+      </c>
+      <c r="H20" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="39"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="143"/>
+      <c r="L20" s="61"/>
+    </row>
+    <row r="21" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A21" s="60"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="68">
+        <v>4</v>
+      </c>
+      <c r="H21" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="39"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="143"/>
+      <c r="L21" s="61"/>
+    </row>
+    <row r="22" spans="1:12" ht="19.5" customHeight="1">
+      <c r="A22" s="60"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="143"/>
+      <c r="L22" s="61"/>
+    </row>
+    <row r="23" spans="1:12" ht="19.5" customHeight="1">
+      <c r="A23" s="48"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="143"/>
+      <c r="L23" s="61"/>
+    </row>
+    <row r="24" spans="1:12" ht="18" customHeight="1" thickBot="1">
+      <c r="A24" s="49"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="144"/>
+      <c r="L24" s="70"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A25" s="98" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="76"/>
+      <c r="C25" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="78" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="99">
+        <v>1</v>
+      </c>
+      <c r="H25" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="100"/>
+      <c r="K25" s="101" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" s="112" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="24" customHeight="1">
+      <c r="A26" s="101"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="102" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="103">
+        <v>2</v>
+      </c>
+      <c r="H26" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="I26" s="45"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="101"/>
+      <c r="L26" s="101"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A27" s="101"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="103">
+        <v>3</v>
+      </c>
+      <c r="H27" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" s="45"/>
+      <c r="J27" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27" s="101"/>
+      <c r="L27" s="101"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A28" s="101"/>
+      <c r="B28" s="86" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="105">
+        <v>4</v>
+      </c>
+      <c r="H28" s="106" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="45"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="101"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A29" s="101"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="105">
+        <v>4</v>
+      </c>
+      <c r="H29" s="106" t="s">
+        <v>64</v>
+      </c>
+      <c r="I29" s="45"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="101"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A30" s="101"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="105">
+        <v>5</v>
+      </c>
+      <c r="H30" s="106" t="s">
+        <v>65</v>
+      </c>
+      <c r="I30" s="45"/>
+      <c r="J30" s="100"/>
+      <c r="K30" s="101"/>
+      <c r="L30" s="101"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A31" s="101"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="105">
+        <v>6</v>
+      </c>
+      <c r="H31" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="I31" s="45"/>
+      <c r="J31" s="100"/>
+      <c r="K31" s="101"/>
+      <c r="L31" s="101"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A32" s="101"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="81"/>
+      <c r="G32" s="105"/>
+      <c r="H32" s="88"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="101"/>
+      <c r="L32" s="101"/>
+    </row>
+    <row r="33" spans="1:12" ht="51.75" customHeight="1">
+      <c r="A33" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="76"/>
+      <c r="C33" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="108"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="79">
+        <v>1</v>
+      </c>
+      <c r="H33" s="83" t="s">
+        <v>52</v>
+      </c>
+      <c r="I33" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33" s="112" t="s">
+        <v>30</v>
+      </c>
+      <c r="L33" s="112" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="30" customHeight="1">
+      <c r="A34" s="60"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" s="82">
+        <v>2</v>
+      </c>
+      <c r="H34" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="101"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A35" s="60"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="91"/>
+      <c r="G35" s="82">
+        <v>3</v>
+      </c>
+      <c r="H35" s="83" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="101"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A36" s="60"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="91"/>
+      <c r="G36" s="87">
+        <v>4</v>
+      </c>
+      <c r="H36" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="101"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A37" s="60"/>
+      <c r="B37" s="86" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="36"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="91"/>
+      <c r="G37" s="87">
+        <v>5</v>
+      </c>
+      <c r="H37" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="36"/>
+      <c r="L37" s="101"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A38" s="60"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="87">
+        <v>6</v>
+      </c>
+      <c r="H38" s="106" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="101"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A39" s="60"/>
+      <c r="B39" s="80"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="87"/>
+      <c r="H39" s="106" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="101"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A40" s="60"/>
+      <c r="B40" s="80"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="88"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="101"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A41" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="109" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="56"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="58">
+        <v>1</v>
+      </c>
+      <c r="H41" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="I41" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="J41" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="K41" s="145" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="146" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="27.75" customHeight="1">
+      <c r="A42" s="60"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="64">
+        <v>2</v>
+      </c>
+      <c r="H42" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="I42" s="39"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="143"/>
+      <c r="L42" s="61"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A43" s="60"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="65">
+        <v>3</v>
+      </c>
+      <c r="H43" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="I43" s="39"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="143"/>
+      <c r="L43" s="61"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A44" s="60"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" s="68">
+        <v>4</v>
+      </c>
+      <c r="H44" s="94" t="s">
+        <v>84</v>
+      </c>
+      <c r="I44" s="39"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="143"/>
+      <c r="L44" s="61"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A45" s="60"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="63"/>
+      <c r="G45" s="68">
+        <v>5</v>
+      </c>
+      <c r="H45" s="94" t="s">
+        <v>85</v>
+      </c>
+      <c r="I45" s="39"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="143"/>
+      <c r="L45" s="61"/>
+    </row>
+    <row r="46" spans="1:12" ht="52.5" customHeight="1" thickBot="1">
+      <c r="A46" s="49"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="70"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="110">
+        <v>6</v>
+      </c>
+      <c r="H46" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="I46" s="47"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="144"/>
+      <c r="L46" s="70"/>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A47" s="112" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="76"/>
+      <c r="C47" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="J4" s="84" t="s">
+      <c r="D47" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="59" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="60" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="32.25" customHeight="1">
-      <c r="A5" s="64"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13">
-        <v>2</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="64"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-    </row>
-    <row r="7" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A7" s="64"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="104" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="77" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="64"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-    </row>
-    <row r="9" spans="1:12" ht="38.25" customHeight="1" thickBot="1">
-      <c r="A9" s="65"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="86" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="98" t="s">
-        <v>131</v>
-      </c>
-      <c r="E10" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="22">
+      <c r="E47" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" s="99">
         <v>1</v>
       </c>
-      <c r="H10" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="87" t="s">
-        <v>133</v>
-      </c>
-      <c r="J10" s="87" t="s">
-        <v>134</v>
-      </c>
-      <c r="K10" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="45.75" thickBot="1">
-      <c r="A11" s="64"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="24">
-        <v>2</v>
-      </c>
-      <c r="H11" s="91" t="s">
+      <c r="H47" s="106" t="s">
+        <v>52</v>
+      </c>
+      <c r="I47" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="53"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="64"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="100" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="53"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="64"/>
-      <c r="B13" s="85" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="53"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="64"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="53"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="64"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="53"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="64"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="53"/>
-    </row>
-    <row r="17" spans="1:12" ht="7.5" customHeight="1" thickBot="1">
-      <c r="A17" s="64"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="53"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A18" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="10">
-        <v>1</v>
-      </c>
-      <c r="H18" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="84" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" s="119" t="s">
-        <v>69</v>
-      </c>
-      <c r="K18" s="125" t="s">
-        <v>31</v>
-      </c>
-      <c r="L18" s="124" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A19" s="64"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13">
-        <v>2</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="53"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="122"/>
-      <c r="L19" s="57"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A20" s="64"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="78" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="14">
-        <v>3</v>
-      </c>
-      <c r="H20" s="82" t="s">
-        <v>55</v>
-      </c>
-      <c r="I20" s="53"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="122"/>
-      <c r="L20" s="57"/>
-    </row>
-    <row r="21" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A21" s="64"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="15">
-        <v>4</v>
-      </c>
-      <c r="H21" s="83" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="53"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="122"/>
-      <c r="L21" s="57"/>
-    </row>
-    <row r="22" spans="1:12" ht="19.5" customHeight="1">
-      <c r="A22" s="64"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="122"/>
-      <c r="L22" s="57"/>
-    </row>
-    <row r="23" spans="1:12" ht="19.5" customHeight="1">
-      <c r="A23" s="73"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="122"/>
-      <c r="L23" s="57"/>
-    </row>
-    <row r="24" spans="1:12" ht="18" customHeight="1" thickBot="1">
-      <c r="A24" s="65"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="123"/>
-      <c r="L24" s="58"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A25" s="61" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="87" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="87" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="89" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="29">
-        <v>1</v>
-      </c>
-      <c r="H25" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="87" t="s">
-        <v>68</v>
-      </c>
-      <c r="J25" s="30"/>
-      <c r="K25" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="L25" s="97" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="24" customHeight="1">
-      <c r="A26" s="69"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="90" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="31">
-        <v>2</v>
-      </c>
-      <c r="H26" s="91" t="s">
-        <v>62</v>
-      </c>
-      <c r="I26" s="67"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A27" s="69"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="31">
-        <v>3</v>
-      </c>
-      <c r="H27" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="67"/>
-      <c r="J27" s="96" t="s">
-        <v>70</v>
-      </c>
-      <c r="K27" s="69"/>
-      <c r="L27" s="69"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" s="69"/>
-      <c r="B28" s="85" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="32">
-        <v>4</v>
-      </c>
-      <c r="H28" s="93" t="s">
-        <v>64</v>
-      </c>
-      <c r="I28" s="67"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A29" s="69"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="32">
-        <v>4</v>
-      </c>
-      <c r="H29" s="93" t="s">
-        <v>65</v>
-      </c>
-      <c r="I29" s="67"/>
-      <c r="J29" s="96"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A30" s="69"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="32">
-        <v>5</v>
-      </c>
-      <c r="H30" s="93" t="s">
-        <v>66</v>
-      </c>
-      <c r="I30" s="67"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A31" s="69"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="32">
-        <v>6</v>
-      </c>
-      <c r="H31" s="94" t="s">
-        <v>67</v>
-      </c>
-      <c r="I31" s="67"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A32" s="69"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A33" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="86" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="98" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="70"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="22">
-        <v>1</v>
-      </c>
-      <c r="H33" s="91" t="s">
-        <v>53</v>
-      </c>
-      <c r="I33" s="87" t="s">
-        <v>80</v>
-      </c>
-      <c r="J33" s="87" t="s">
-        <v>81</v>
-      </c>
-      <c r="K33" s="97" t="s">
-        <v>31</v>
-      </c>
-      <c r="L33" s="97" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="30" customHeight="1">
-      <c r="A34" s="64"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="78" t="s">
-        <v>73</v>
-      </c>
-      <c r="G34" s="24">
-        <v>2</v>
-      </c>
-      <c r="H34" s="91" t="s">
-        <v>62</v>
-      </c>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="69"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A35" s="64"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="24">
-        <v>3</v>
-      </c>
-      <c r="H35" s="91" t="s">
-        <v>74</v>
-      </c>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="69"/>
-    </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A36" s="64"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="71"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="26">
-        <v>4</v>
-      </c>
-      <c r="H36" s="92" t="s">
-        <v>75</v>
-      </c>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="69"/>
-    </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A37" s="64"/>
-      <c r="B37" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="90" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="78"/>
-      <c r="G37" s="26">
-        <v>5</v>
-      </c>
-      <c r="H37" s="93" t="s">
-        <v>76</v>
-      </c>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="69"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A38" s="64"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="77"/>
-      <c r="G38" s="26">
-        <v>6</v>
-      </c>
-      <c r="H38" s="93" t="s">
-        <v>77</v>
-      </c>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="69"/>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A39" s="64"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="69"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A40" s="64"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="72"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="69"/>
-    </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A41" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="102" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" s="103" t="s">
-        <v>83</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="10">
-        <v>1</v>
-      </c>
-      <c r="H41" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="I41" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="J41" s="119" t="s">
-        <v>88</v>
-      </c>
-      <c r="K41" s="121" t="s">
-        <v>31</v>
-      </c>
-      <c r="L41" s="120" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="27.75" customHeight="1">
-      <c r="A42" s="64"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="13">
-        <v>2</v>
-      </c>
-      <c r="H42" s="80" t="s">
-        <v>62</v>
-      </c>
-      <c r="I42" s="53"/>
-      <c r="J42" s="73"/>
-      <c r="K42" s="122"/>
-      <c r="L42" s="57"/>
-    </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A43" s="64"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="14">
-        <v>3</v>
-      </c>
-      <c r="H43" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="I43" s="53"/>
-      <c r="J43" s="73"/>
-      <c r="K43" s="122"/>
-      <c r="L43" s="57"/>
-    </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A44" s="64"/>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="77" t="s">
-        <v>50</v>
-      </c>
-      <c r="G44" s="15">
-        <v>4</v>
-      </c>
-      <c r="H44" s="83" t="s">
-        <v>85</v>
-      </c>
-      <c r="I44" s="53"/>
-      <c r="J44" s="73"/>
-      <c r="K44" s="122"/>
-      <c r="L44" s="57"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A45" s="64"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="104" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="12"/>
-      <c r="G45" s="15">
-        <v>5</v>
-      </c>
-      <c r="H45" s="83" t="s">
-        <v>86</v>
-      </c>
-      <c r="I45" s="53"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="122"/>
-      <c r="L45" s="57"/>
-    </row>
-    <row r="46" spans="1:12" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A46" s="65"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="105">
-        <v>6</v>
-      </c>
-      <c r="H46" s="106" t="s">
-        <v>67</v>
-      </c>
-      <c r="I46" s="54"/>
-      <c r="J46" s="65"/>
-      <c r="K46" s="123"/>
-      <c r="L46" s="58"/>
-    </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A47" s="97" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="86" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="87" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" s="87" t="s">
-        <v>50</v>
-      </c>
-      <c r="F47" s="89" t="s">
-        <v>91</v>
-      </c>
-      <c r="G47" s="29">
-        <v>1</v>
-      </c>
-      <c r="H47" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="I47" s="87" t="s">
-        <v>104</v>
-      </c>
-      <c r="J47" s="30"/>
+      <c r="J47" s="100"/>
       <c r="K47" s="113" t="s">
-        <v>31</v>
-      </c>
-      <c r="L47" s="97" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="L47" s="112" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1">
       <c r="A48" s="113"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="114"/>
-      <c r="D48" s="115"/>
-      <c r="E48" s="115"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="116">
+      <c r="B48" s="80"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="102"/>
+      <c r="G48" s="114">
         <v>2</v>
       </c>
-      <c r="H48" s="93" t="s">
-        <v>108</v>
-      </c>
-      <c r="I48" s="115"/>
-      <c r="J48" s="88"/>
+      <c r="H48" s="106" t="s">
+        <v>102</v>
+      </c>
+      <c r="I48" s="44"/>
+      <c r="J48" s="27"/>
       <c r="K48" s="113"/>
       <c r="L48" s="113"/>
     </row>
     <row r="49" spans="1:12" ht="36" customHeight="1">
-      <c r="A49" s="69"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="68"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="67"/>
-      <c r="F49" s="90" t="s">
+      <c r="A49" s="101"/>
+      <c r="B49" s="80"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="102" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" s="115">
+        <v>3</v>
+      </c>
+      <c r="H49" s="116" t="s">
+        <v>130</v>
+      </c>
+      <c r="I49" s="45"/>
+      <c r="J49" s="100"/>
+      <c r="K49" s="101"/>
+      <c r="L49" s="101"/>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A50" s="101"/>
+      <c r="B50" s="80"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="102" t="s">
+        <v>131</v>
+      </c>
+      <c r="G50" s="117"/>
+      <c r="H50" s="118"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="100"/>
+      <c r="K50" s="101"/>
+      <c r="L50" s="101"/>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A51" s="101"/>
+      <c r="B51" s="80"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="102" t="s">
+        <v>90</v>
+      </c>
+      <c r="G51" s="105">
+        <v>4</v>
+      </c>
+      <c r="H51" s="106" t="s">
+        <v>77</v>
+      </c>
+      <c r="I51" s="45"/>
+      <c r="J51" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="K51" s="101"/>
+      <c r="L51" s="101"/>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A52" s="101"/>
+      <c r="B52" s="86" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="102" t="s">
+        <v>91</v>
+      </c>
+      <c r="G52" s="105"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="101"/>
+      <c r="L52" s="101"/>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A53" s="101"/>
+      <c r="B53" s="80"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="G49" s="111">
+      <c r="G53" s="105"/>
+      <c r="H53" s="88"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="44"/>
+      <c r="K53" s="101"/>
+      <c r="L53" s="101"/>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A54" s="101"/>
+      <c r="B54" s="80"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54" s="105"/>
+      <c r="H54" s="89"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="100"/>
+      <c r="K54" s="101"/>
+      <c r="L54" s="101"/>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A55" s="101"/>
+      <c r="B55" s="80"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="G55" s="119"/>
+      <c r="H55" s="89"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="101"/>
+      <c r="L55" s="101"/>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A56" s="101"/>
+      <c r="B56" s="80"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="G56" s="119"/>
+      <c r="H56" s="89"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="101"/>
+      <c r="L56" s="101"/>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A57" s="101"/>
+      <c r="B57" s="80"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="102" t="s">
+        <v>96</v>
+      </c>
+      <c r="G57" s="119"/>
+      <c r="H57" s="89"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="101"/>
+      <c r="L57" s="101"/>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A58" s="101"/>
+      <c r="B58" s="80"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="102" t="s">
+        <v>97</v>
+      </c>
+      <c r="G58" s="119"/>
+      <c r="H58" s="89"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="27"/>
+      <c r="K58" s="101"/>
+      <c r="L58" s="101"/>
+    </row>
+    <row r="59" spans="1:12" ht="33" customHeight="1" thickBot="1">
+      <c r="A59" s="101"/>
+      <c r="B59" s="80"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="102" t="s">
+        <v>98</v>
+      </c>
+      <c r="G59" s="105"/>
+      <c r="H59" s="88"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="120"/>
+      <c r="K59" s="101"/>
+      <c r="L59" s="101"/>
+    </row>
+    <row r="60" spans="1:12" ht="37.5" customHeight="1">
+      <c r="A60" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="76"/>
+      <c r="C60" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D60" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60" s="108"/>
+      <c r="F60" s="121"/>
+      <c r="G60" s="79">
+        <v>1</v>
+      </c>
+      <c r="H60" s="104" t="s">
+        <v>52</v>
+      </c>
+      <c r="I60" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="J60" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="K60" s="112" t="s">
+        <v>30</v>
+      </c>
+      <c r="L60" s="147" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A61" s="60"/>
+      <c r="B61" s="80"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="81"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="82">
+        <v>2</v>
+      </c>
+      <c r="H61" s="104" t="s">
+        <v>102</v>
+      </c>
+      <c r="I61" s="39"/>
+      <c r="J61" s="36"/>
+      <c r="K61" s="113"/>
+      <c r="L61" s="36"/>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A62" s="60"/>
+      <c r="B62" s="80"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="81"/>
+      <c r="F62" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="G62" s="82">
         <v>3</v>
       </c>
-      <c r="H49" s="109" t="s">
-        <v>103</v>
-      </c>
-      <c r="I49" s="67"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="69"/>
-      <c r="L49" s="69"/>
-    </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A50" s="69"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="68"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="90" t="s">
-        <v>93</v>
-      </c>
-      <c r="G50" s="112"/>
-      <c r="H50" s="110"/>
-      <c r="I50" s="67"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="69"/>
-      <c r="L50" s="69"/>
-    </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A51" s="69"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="68"/>
-      <c r="D51" s="67"/>
-      <c r="E51" s="67"/>
-      <c r="F51" s="90" t="s">
-        <v>94</v>
-      </c>
-      <c r="G51" s="32">
+      <c r="H62" s="104" t="s">
+        <v>77</v>
+      </c>
+      <c r="I62" s="39"/>
+      <c r="J62" s="36"/>
+      <c r="K62" s="101"/>
+      <c r="L62" s="36"/>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A63" s="60"/>
+      <c r="B63" s="80"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="102" t="s">
+        <v>49</v>
+      </c>
+      <c r="F63" s="63"/>
+      <c r="G63" s="87"/>
+      <c r="H63" s="88"/>
+      <c r="I63" s="39"/>
+      <c r="J63" s="36"/>
+      <c r="K63" s="101"/>
+      <c r="L63" s="36"/>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A64" s="60"/>
+      <c r="B64" s="86" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="36"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="81"/>
+      <c r="F64" s="63"/>
+      <c r="G64" s="87"/>
+      <c r="H64" s="88"/>
+      <c r="I64" s="39"/>
+      <c r="J64" s="36"/>
+      <c r="K64" s="101"/>
+      <c r="L64" s="36"/>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A65" s="60"/>
+      <c r="B65" s="80"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="61"/>
+      <c r="E65" s="81"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="87"/>
+      <c r="H65" s="88"/>
+      <c r="I65" s="39"/>
+      <c r="J65" s="36"/>
+      <c r="K65" s="101"/>
+      <c r="L65" s="36"/>
+    </row>
+    <row r="66" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A66" s="60"/>
+      <c r="B66" s="80"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="81"/>
+      <c r="F66" s="63"/>
+      <c r="G66" s="87"/>
+      <c r="H66" s="89"/>
+      <c r="I66" s="39"/>
+      <c r="J66" s="36"/>
+      <c r="K66" s="101"/>
+      <c r="L66" s="36"/>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A67" s="60"/>
+      <c r="B67" s="80"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="90"/>
+      <c r="F67" s="72"/>
+      <c r="G67" s="87"/>
+      <c r="H67" s="88"/>
+      <c r="I67" s="39"/>
+      <c r="J67" s="36"/>
+      <c r="K67" s="101"/>
+      <c r="L67" s="36"/>
+    </row>
+    <row r="68" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A68" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" s="109" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D68" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="E68" s="56"/>
+      <c r="F68" s="57"/>
+      <c r="G68" s="58">
+        <v>1</v>
+      </c>
+      <c r="H68" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="I68" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="J68" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="K68" s="112" t="s">
+        <v>30</v>
+      </c>
+      <c r="L68" s="148" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A69" s="60"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="61"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="63"/>
+      <c r="G69" s="64">
+        <v>2</v>
+      </c>
+      <c r="H69" s="122" t="s">
+        <v>114</v>
+      </c>
+      <c r="I69" s="39"/>
+      <c r="J69" s="36"/>
+      <c r="K69" s="101"/>
+      <c r="L69" s="36"/>
+    </row>
+    <row r="70" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A70" s="60"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="61"/>
+      <c r="E70" s="123" t="s">
+        <v>49</v>
+      </c>
+      <c r="F70" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="G70" s="65"/>
+      <c r="H70" s="64"/>
+      <c r="I70" s="39"/>
+      <c r="J70" s="36"/>
+      <c r="K70" s="101"/>
+      <c r="L70" s="36"/>
+    </row>
+    <row r="71" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A71" s="60"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="61"/>
+      <c r="E71" s="62"/>
+      <c r="F71" s="63"/>
+      <c r="G71" s="68"/>
+      <c r="H71" s="69"/>
+      <c r="I71" s="39"/>
+      <c r="J71" s="36"/>
+      <c r="K71" s="101"/>
+      <c r="L71" s="36"/>
+    </row>
+    <row r="72" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A72" s="60"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="62"/>
+      <c r="F72" s="63"/>
+      <c r="G72" s="68"/>
+      <c r="H72" s="69"/>
+      <c r="I72" s="39"/>
+      <c r="J72" s="36"/>
+      <c r="K72" s="101"/>
+      <c r="L72" s="36"/>
+    </row>
+    <row r="73" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A73" s="48"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="61"/>
+      <c r="E73" s="95"/>
+      <c r="F73" s="63"/>
+      <c r="G73" s="96"/>
+      <c r="H73" s="124"/>
+      <c r="I73" s="40"/>
+      <c r="J73" s="37"/>
+      <c r="K73" s="101"/>
+      <c r="L73" s="37"/>
+    </row>
+    <row r="74" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A74" s="125" t="s">
+        <v>46</v>
+      </c>
+      <c r="B74" s="126"/>
+      <c r="C74" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D74" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="E74" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F74" s="127" t="s">
+        <v>107</v>
+      </c>
+      <c r="G74" s="128">
+        <v>1</v>
+      </c>
+      <c r="H74" s="129" t="s">
+        <v>52</v>
+      </c>
+      <c r="I74" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="J74" s="130"/>
+      <c r="K74" s="149" t="s">
+        <v>30</v>
+      </c>
+      <c r="L74" s="150" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="27.75" customHeight="1">
+      <c r="A75" s="131"/>
+      <c r="B75" s="80"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="81"/>
+      <c r="G75" s="132">
+        <v>2</v>
+      </c>
+      <c r="H75" s="83" t="s">
+        <v>109</v>
+      </c>
+      <c r="I75" s="40"/>
+      <c r="J75" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="K75" s="101"/>
+      <c r="L75" s="151"/>
+    </row>
+    <row r="76" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A76" s="131"/>
+      <c r="B76" s="80"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="102" t="s">
+        <v>108</v>
+      </c>
+      <c r="G76" s="132">
+        <v>3</v>
+      </c>
+      <c r="H76" s="104" t="s">
+        <v>110</v>
+      </c>
+      <c r="I76" s="40"/>
+      <c r="J76" s="44"/>
+      <c r="K76" s="101"/>
+      <c r="L76" s="151"/>
+    </row>
+    <row r="77" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A77" s="131"/>
+      <c r="B77" s="80"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="81"/>
+      <c r="G77" s="119">
         <v>4</v>
       </c>
-      <c r="H51" s="93" t="s">
-        <v>78</v>
-      </c>
-      <c r="I51" s="67"/>
-      <c r="J51" s="96" t="s">
-        <v>105</v>
-      </c>
-      <c r="K51" s="69"/>
-      <c r="L51" s="69"/>
-    </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A52" s="69"/>
-      <c r="B52" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" s="68"/>
-      <c r="D52" s="67"/>
-      <c r="E52" s="67"/>
-      <c r="F52" s="90" t="s">
-        <v>95</v>
-      </c>
-      <c r="G52" s="32"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="67"/>
-      <c r="J52" s="96"/>
-      <c r="K52" s="69"/>
-      <c r="L52" s="69"/>
-    </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A53" s="69"/>
-      <c r="B53" s="23"/>
-      <c r="C53" s="68"/>
-      <c r="D53" s="67"/>
-      <c r="E53" s="67"/>
-      <c r="F53" s="90" t="s">
-        <v>96</v>
-      </c>
-      <c r="G53" s="32"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="67"/>
-      <c r="J53" s="96"/>
-      <c r="K53" s="69"/>
-      <c r="L53" s="69"/>
-    </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A54" s="69"/>
-      <c r="B54" s="23"/>
-      <c r="C54" s="68"/>
-      <c r="D54" s="67"/>
-      <c r="E54" s="67"/>
-      <c r="F54" s="90" t="s">
-        <v>97</v>
-      </c>
-      <c r="G54" s="32"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="67"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="69"/>
-      <c r="L54" s="69"/>
-    </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A55" s="69"/>
-      <c r="B55" s="23"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="67"/>
-      <c r="F55" s="90" t="s">
-        <v>98</v>
-      </c>
-      <c r="G55" s="108"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="67"/>
-      <c r="J55" s="88"/>
-      <c r="K55" s="69"/>
-      <c r="L55" s="69"/>
-    </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A56" s="69"/>
-      <c r="B56" s="23"/>
-      <c r="C56" s="68"/>
-      <c r="D56" s="67"/>
-      <c r="E56" s="67"/>
-      <c r="F56" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="G56" s="108"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="67"/>
-      <c r="J56" s="88"/>
-      <c r="K56" s="69"/>
-      <c r="L56" s="69"/>
-    </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A57" s="69"/>
-      <c r="B57" s="23"/>
-      <c r="C57" s="68"/>
-      <c r="D57" s="67"/>
-      <c r="E57" s="67"/>
-      <c r="F57" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="G57" s="108"/>
-      <c r="H57" s="28"/>
-      <c r="I57" s="67"/>
-      <c r="J57" s="88"/>
-      <c r="K57" s="69"/>
-      <c r="L57" s="69"/>
-    </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A58" s="69"/>
-      <c r="B58" s="23"/>
-      <c r="C58" s="68"/>
-      <c r="D58" s="67"/>
-      <c r="E58" s="67"/>
-      <c r="F58" s="90" t="s">
-        <v>101</v>
-      </c>
-      <c r="G58" s="108"/>
-      <c r="H58" s="28"/>
-      <c r="I58" s="67"/>
-      <c r="J58" s="88"/>
-      <c r="K58" s="69"/>
-      <c r="L58" s="69"/>
-    </row>
-    <row r="59" spans="1:12" ht="33" customHeight="1" thickBot="1">
-      <c r="A59" s="69"/>
-      <c r="B59" s="23"/>
-      <c r="C59" s="68"/>
-      <c r="D59" s="67"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="90" t="s">
-        <v>102</v>
-      </c>
-      <c r="G59" s="32"/>
-      <c r="H59" s="27"/>
-      <c r="I59" s="67"/>
-      <c r="J59" s="95"/>
-      <c r="K59" s="69"/>
-      <c r="L59" s="69"/>
-    </row>
-    <row r="60" spans="1:12" ht="37.5" customHeight="1">
-      <c r="A60" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="B60" s="21"/>
-      <c r="C60" s="86" t="s">
-        <v>106</v>
-      </c>
-      <c r="D60" s="98" t="s">
-        <v>107</v>
-      </c>
-      <c r="E60" s="70"/>
-      <c r="F60" s="99"/>
-      <c r="G60" s="22">
-        <v>1</v>
-      </c>
-      <c r="H60" s="92" t="s">
-        <v>53</v>
-      </c>
-      <c r="I60" s="87" t="s">
-        <v>109</v>
-      </c>
-      <c r="J60" s="87" t="s">
-        <v>110</v>
-      </c>
-      <c r="K60" s="97" t="s">
-        <v>31</v>
-      </c>
-      <c r="L60" s="117" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A61" s="64"/>
-      <c r="B61" s="23"/>
-      <c r="C61" s="53"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="71"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="24">
-        <v>2</v>
-      </c>
-      <c r="H61" s="92" t="s">
-        <v>108</v>
-      </c>
-      <c r="I61" s="53"/>
-      <c r="J61" s="53"/>
-      <c r="K61" s="113"/>
-      <c r="L61" s="53"/>
-    </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A62" s="64"/>
-      <c r="B62" s="23"/>
-      <c r="C62" s="53"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="71"/>
-      <c r="F62" s="77" t="s">
-        <v>50</v>
-      </c>
-      <c r="G62" s="24">
-        <v>3</v>
-      </c>
-      <c r="H62" s="92" t="s">
-        <v>78</v>
-      </c>
-      <c r="I62" s="53"/>
-      <c r="J62" s="53"/>
-      <c r="K62" s="69"/>
-      <c r="L62" s="53"/>
-    </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A63" s="64"/>
-      <c r="B63" s="23"/>
-      <c r="C63" s="53"/>
-      <c r="D63" s="57"/>
-      <c r="E63" s="90" t="s">
-        <v>50</v>
-      </c>
-      <c r="F63" s="12"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="27"/>
-      <c r="I63" s="53"/>
-      <c r="J63" s="53"/>
-      <c r="K63" s="69"/>
-      <c r="L63" s="53"/>
-    </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A64" s="64"/>
-      <c r="B64" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C64" s="53"/>
-      <c r="D64" s="57"/>
-      <c r="E64" s="71"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="26"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="53"/>
-      <c r="J64" s="53"/>
-      <c r="K64" s="69"/>
-      <c r="L64" s="53"/>
-    </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A65" s="64"/>
-      <c r="B65" s="23"/>
-      <c r="C65" s="53"/>
-      <c r="D65" s="57"/>
-      <c r="E65" s="71"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="27"/>
-      <c r="I65" s="53"/>
-      <c r="J65" s="53"/>
-      <c r="K65" s="69"/>
-      <c r="L65" s="53"/>
-    </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A66" s="64"/>
-      <c r="B66" s="23"/>
-      <c r="C66" s="53"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="71"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="28"/>
-      <c r="I66" s="53"/>
-      <c r="J66" s="53"/>
-      <c r="K66" s="69"/>
-      <c r="L66" s="53"/>
-    </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A67" s="64"/>
-      <c r="B67" s="23"/>
-      <c r="C67" s="53"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="72"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="53"/>
-      <c r="J67" s="53"/>
-      <c r="K67" s="69"/>
-      <c r="L67" s="53"/>
-    </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A68" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="B68" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="C68" s="102" t="s">
-        <v>120</v>
-      </c>
-      <c r="D68" s="103" t="s">
-        <v>121</v>
-      </c>
-      <c r="E68" s="8"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="10">
-        <v>1</v>
-      </c>
-      <c r="H68" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="I68" s="84" t="s">
-        <v>123</v>
-      </c>
-      <c r="J68" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="K68" s="97" t="s">
-        <v>31</v>
-      </c>
-      <c r="L68" s="107" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A69" s="64"/>
-      <c r="B69" s="53"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="57"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="13">
-        <v>2</v>
-      </c>
-      <c r="H69" s="81" t="s">
-        <v>122</v>
-      </c>
-      <c r="I69" s="53"/>
-      <c r="J69" s="53"/>
-      <c r="K69" s="69"/>
-      <c r="L69" s="53"/>
-    </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A70" s="64"/>
-      <c r="B70" s="53"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="57"/>
-      <c r="E70" s="118" t="s">
-        <v>50</v>
-      </c>
-      <c r="F70" s="77" t="s">
-        <v>50</v>
-      </c>
-      <c r="G70" s="14"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="53"/>
-      <c r="J70" s="53"/>
-      <c r="K70" s="69"/>
-      <c r="L70" s="53"/>
-    </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A71" s="64"/>
-      <c r="B71" s="53"/>
-      <c r="C71" s="53"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="15"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="53"/>
-      <c r="J71" s="53"/>
-      <c r="K71" s="69"/>
-      <c r="L71" s="53"/>
-    </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A72" s="64"/>
-      <c r="B72" s="53"/>
-      <c r="C72" s="53"/>
-      <c r="D72" s="57"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="16"/>
-      <c r="I72" s="53"/>
-      <c r="J72" s="53"/>
-      <c r="K72" s="69"/>
-      <c r="L72" s="53"/>
-    </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A73" s="73"/>
-      <c r="B73" s="74"/>
-      <c r="C73" s="74"/>
-      <c r="D73" s="57"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="76"/>
-      <c r="H73" s="126"/>
-      <c r="I73" s="74"/>
-      <c r="J73" s="74"/>
-      <c r="K73" s="69"/>
-      <c r="L73" s="74"/>
-    </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A74" s="127" t="s">
-        <v>47</v>
-      </c>
-      <c r="B74" s="128"/>
-      <c r="C74" s="129" t="s">
+      <c r="H77" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="D74" s="130" t="s">
-        <v>112</v>
-      </c>
-      <c r="E74" s="130" t="s">
-        <v>50</v>
-      </c>
-      <c r="F74" s="131" t="s">
-        <v>113</v>
-      </c>
-      <c r="G74" s="132">
-        <v>1</v>
-      </c>
-      <c r="H74" s="133" t="s">
-        <v>53</v>
-      </c>
-      <c r="I74" s="130" t="s">
-        <v>118</v>
-      </c>
-      <c r="J74" s="134"/>
-      <c r="K74" s="135" t="s">
-        <v>31</v>
-      </c>
-      <c r="L74" s="136" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="27.75" customHeight="1">
-      <c r="A75" s="137"/>
-      <c r="B75" s="23"/>
-      <c r="C75" s="68"/>
-      <c r="D75" s="67"/>
-      <c r="E75" s="67"/>
-      <c r="F75" s="71"/>
-      <c r="G75" s="138">
-        <v>2</v>
-      </c>
-      <c r="H75" s="91" t="s">
-        <v>115</v>
-      </c>
-      <c r="I75" s="74"/>
-      <c r="J75" s="88"/>
-      <c r="K75" s="69"/>
-      <c r="L75" s="139"/>
-    </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A76" s="137"/>
-      <c r="B76" s="23"/>
-      <c r="C76" s="68"/>
-      <c r="D76" s="67"/>
-      <c r="E76" s="67"/>
-      <c r="F76" s="90" t="s">
-        <v>114</v>
-      </c>
-      <c r="G76" s="138">
-        <v>3</v>
-      </c>
-      <c r="H76" s="92" t="s">
-        <v>116</v>
-      </c>
-      <c r="I76" s="74"/>
-      <c r="J76" s="88"/>
-      <c r="K76" s="69"/>
-      <c r="L76" s="139"/>
-    </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A77" s="137"/>
-      <c r="B77" s="23"/>
-      <c r="C77" s="68"/>
-      <c r="D77" s="67"/>
-      <c r="E77" s="67"/>
-      <c r="F77" s="71"/>
-      <c r="G77" s="108">
-        <v>4</v>
-      </c>
-      <c r="H77" s="93" t="s">
-        <v>117</v>
-      </c>
-      <c r="I77" s="74"/>
-      <c r="J77" s="140" t="s">
-        <v>119</v>
-      </c>
-      <c r="K77" s="69"/>
-      <c r="L77" s="139"/>
+      <c r="I77" s="40"/>
+      <c r="J77" s="44"/>
+      <c r="K77" s="101"/>
+      <c r="L77" s="151"/>
     </row>
     <row r="78" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A78" s="137"/>
-      <c r="B78" s="23"/>
-      <c r="C78" s="68"/>
-      <c r="D78" s="67"/>
-      <c r="E78" s="67"/>
-      <c r="F78" s="71"/>
-      <c r="G78" s="108"/>
-      <c r="H78" s="27"/>
-      <c r="I78" s="74"/>
-      <c r="J78" s="88"/>
-      <c r="K78" s="69"/>
-      <c r="L78" s="139"/>
+      <c r="A78" s="131"/>
+      <c r="B78" s="80"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="30"/>
+      <c r="F78" s="81"/>
+      <c r="G78" s="119"/>
+      <c r="H78" s="88"/>
+      <c r="I78" s="40"/>
+      <c r="J78" s="44"/>
+      <c r="K78" s="101"/>
+      <c r="L78" s="151"/>
     </row>
     <row r="79" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A79" s="137"/>
-      <c r="B79" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C79" s="68"/>
-      <c r="D79" s="67"/>
-      <c r="E79" s="67"/>
-      <c r="F79" s="71"/>
-      <c r="G79" s="108"/>
-      <c r="H79" s="27"/>
-      <c r="I79" s="74"/>
-      <c r="J79" s="88"/>
-      <c r="K79" s="69"/>
-      <c r="L79" s="139"/>
+      <c r="A79" s="131"/>
+      <c r="B79" s="86" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="81"/>
+      <c r="G79" s="119"/>
+      <c r="H79" s="88"/>
+      <c r="I79" s="40"/>
+      <c r="J79" s="44"/>
+      <c r="K79" s="101"/>
+      <c r="L79" s="151"/>
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A80" s="137"/>
-      <c r="B80" s="23"/>
-      <c r="C80" s="68"/>
-      <c r="D80" s="67"/>
-      <c r="E80" s="67"/>
-      <c r="F80" s="71"/>
-      <c r="G80" s="108"/>
-      <c r="H80" s="28"/>
-      <c r="I80" s="74"/>
-      <c r="J80" s="88"/>
-      <c r="K80" s="69"/>
-      <c r="L80" s="139"/>
+      <c r="A80" s="131"/>
+      <c r="B80" s="80"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="81"/>
+      <c r="G80" s="119"/>
+      <c r="H80" s="89"/>
+      <c r="I80" s="40"/>
+      <c r="J80" s="27"/>
+      <c r="K80" s="101"/>
+      <c r="L80" s="151"/>
     </row>
     <row r="81" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A81" s="141"/>
-      <c r="B81" s="142"/>
-      <c r="C81" s="143"/>
-      <c r="D81" s="144"/>
-      <c r="E81" s="144"/>
-      <c r="F81" s="145"/>
-      <c r="G81" s="146"/>
-      <c r="H81" s="147"/>
-      <c r="I81" s="148"/>
-      <c r="J81" s="149"/>
-      <c r="K81" s="150"/>
-      <c r="L81" s="151"/>
+      <c r="A81" s="133"/>
+      <c r="B81" s="134"/>
+      <c r="C81" s="31"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="135"/>
+      <c r="G81" s="136"/>
+      <c r="H81" s="137"/>
+      <c r="I81" s="42"/>
+      <c r="J81" s="28"/>
+      <c r="K81" s="152"/>
+      <c r="L81" s="153"/>
     </row>
     <row r="82" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="83" spans="1:12" ht="15.75" customHeight="1"/>
@@ -4423,12 +4501,68 @@
     <row r="989" ht="15.75" customHeight="1"/>
     <row r="990" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="80">
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="G49:G50"/>
+  <mergeCells count="83">
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="J75:J79"/>
+    <mergeCell ref="K4:K9"/>
+    <mergeCell ref="L4:L9"/>
+    <mergeCell ref="K10:K17"/>
+    <mergeCell ref="L10:L17"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="I10:I17"/>
+    <mergeCell ref="J10:J17"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="D4:D9"/>
+    <mergeCell ref="I4:I9"/>
+    <mergeCell ref="J4:J9"/>
+    <mergeCell ref="E10:E16"/>
+    <mergeCell ref="K25:K32"/>
+    <mergeCell ref="L25:L32"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="D18:D24"/>
+    <mergeCell ref="K18:K24"/>
+    <mergeCell ref="L18:L24"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="J18:J24"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="C25:C32"/>
+    <mergeCell ref="D25:D32"/>
+    <mergeCell ref="E25:E32"/>
+    <mergeCell ref="I18:I24"/>
+    <mergeCell ref="I25:I32"/>
+    <mergeCell ref="K33:K40"/>
+    <mergeCell ref="L33:L40"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="D41:D46"/>
+    <mergeCell ref="I41:I46"/>
+    <mergeCell ref="J41:J46"/>
+    <mergeCell ref="K41:K46"/>
+    <mergeCell ref="L41:L46"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="C33:C40"/>
+    <mergeCell ref="D33:D40"/>
+    <mergeCell ref="I33:I40"/>
+    <mergeCell ref="J33:J40"/>
+    <mergeCell ref="K47:K59"/>
+    <mergeCell ref="L47:L59"/>
+    <mergeCell ref="A60:A67"/>
+    <mergeCell ref="C60:C67"/>
+    <mergeCell ref="D60:D67"/>
+    <mergeCell ref="I60:I67"/>
+    <mergeCell ref="J60:J67"/>
+    <mergeCell ref="K60:K67"/>
+    <mergeCell ref="L60:L67"/>
+    <mergeCell ref="A47:A59"/>
+    <mergeCell ref="C47:C59"/>
+    <mergeCell ref="D47:D59"/>
+    <mergeCell ref="E47:E59"/>
     <mergeCell ref="J51:J53"/>
     <mergeCell ref="J68:J73"/>
     <mergeCell ref="K68:K73"/>
@@ -4445,65 +4579,12 @@
     <mergeCell ref="C68:C73"/>
     <mergeCell ref="D68:D73"/>
     <mergeCell ref="I68:I73"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="G49:G50"/>
     <mergeCell ref="I47:I59"/>
-    <mergeCell ref="K47:K59"/>
-    <mergeCell ref="L47:L59"/>
-    <mergeCell ref="A60:A67"/>
-    <mergeCell ref="C60:C67"/>
-    <mergeCell ref="D60:D67"/>
-    <mergeCell ref="I60:I67"/>
-    <mergeCell ref="J60:J67"/>
-    <mergeCell ref="K60:K67"/>
-    <mergeCell ref="L60:L67"/>
-    <mergeCell ref="A47:A59"/>
-    <mergeCell ref="C47:C59"/>
-    <mergeCell ref="D47:D59"/>
-    <mergeCell ref="E47:E59"/>
-    <mergeCell ref="K33:K40"/>
-    <mergeCell ref="L33:L40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="D41:D46"/>
-    <mergeCell ref="I41:I46"/>
-    <mergeCell ref="J41:J46"/>
-    <mergeCell ref="K41:K46"/>
-    <mergeCell ref="L41:L46"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="C33:C40"/>
-    <mergeCell ref="D33:D40"/>
-    <mergeCell ref="I33:I40"/>
-    <mergeCell ref="J33:J40"/>
-    <mergeCell ref="K25:K32"/>
-    <mergeCell ref="L25:L32"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="D18:D24"/>
-    <mergeCell ref="K18:K24"/>
-    <mergeCell ref="L18:L24"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="J18:J24"/>
-    <mergeCell ref="C18:C24"/>
-    <mergeCell ref="C25:C32"/>
-    <mergeCell ref="D25:D32"/>
-    <mergeCell ref="E25:E32"/>
-    <mergeCell ref="I18:I24"/>
-    <mergeCell ref="I25:I32"/>
-    <mergeCell ref="K4:K9"/>
-    <mergeCell ref="L4:L9"/>
-    <mergeCell ref="K10:K17"/>
-    <mergeCell ref="L10:L17"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="I10:I17"/>
-    <mergeCell ref="J10:J17"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="C4:C9"/>
-    <mergeCell ref="D4:D9"/>
-    <mergeCell ref="I4:I9"/>
-    <mergeCell ref="J4:J9"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4546,160 +4627,160 @@
     <row r="1" spans="2:3" hidden="1"/>
     <row r="2" spans="2:3" hidden="1"/>
     <row r="3" spans="2:3" hidden="1">
-      <c r="B3" s="33"/>
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="2:3" hidden="1">
-      <c r="B4" s="33"/>
+      <c r="B4" s="8"/>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="33"/>
+      <c r="B5" s="8"/>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="35" t="s">
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="35" t="s">
+    <row r="8" spans="2:3" ht="26.25">
+      <c r="B8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="26.25">
-      <c r="B8" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="35" t="s">
+    <row r="9" spans="2:3">
+      <c r="B9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="37" t="s">
+    <row r="10" spans="2:3" ht="26.25">
+      <c r="B10" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" ht="26.25">
-      <c r="B10" s="34" t="s">
+      <c r="C10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="35" t="s">
+    </row>
+    <row r="11" spans="2:3" ht="72" customHeight="1">
+      <c r="B11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="72" customHeight="1">
-      <c r="B11" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="37" t="s">
+    <row r="12" spans="2:3">
+      <c r="B12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="37" t="s">
+    <row r="13" spans="2:3">
+      <c r="B13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="37" t="s">
+    <row r="14" spans="2:3">
+      <c r="B14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="34" t="s">
+    <row r="15" spans="2:3">
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="54" customHeight="1">
+      <c r="B19" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="36" customHeight="1">
+      <c r="B20" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="36" customHeight="1">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B22" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="33" customHeight="1">
+      <c r="B23" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="30" customHeight="1">
+      <c r="B24" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-    </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="54" customHeight="1">
-      <c r="B19" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="36" customHeight="1">
-      <c r="B20" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="36" customHeight="1">
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B22" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="33" customHeight="1">
-      <c r="B23" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="49" t="s">
+      <c r="C24" s="26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="30" customHeight="1">
-      <c r="B24" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="51" t="s">
+    <row r="25" spans="2:3" ht="33.75" customHeight="1">
+      <c r="B25" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="26" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="33.75" customHeight="1">
-      <c r="B25" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="51" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15.75" customHeight="1"/>

</xml_diff>